<commit_message>
Fixed case on serviceId
</commit_message>
<xml_diff>
--- a/src/DID-URL-Low-level-Use Cases 0.2.xlsx
+++ b/src/DID-URL-Low-level-Use Cases 0.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\INDY\did-url-spec\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8125BEA7-BA10-45C5-8DB8-1B3030C6995A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F49027C-AC9C-479D-A03A-FDD99DE727D2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{55C97778-1C7A-4748-8CBF-F07099F47EAB}"/>
   </bookViews>
@@ -192,18 +192,9 @@
     <t>2c2</t>
   </si>
   <si>
-    <t>Transform the DID URL using corresponding service endpoint using "!" transformer (pipe) character and $serviceid transformation option (no parameters)</t>
-  </si>
-  <si>
-    <t>Transform the DID URL using corresponding service endpoint using "!" pipe character and $serviceid transformation option (w/parameters)</t>
-  </si>
-  <si>
     <t>2d2</t>
   </si>
   <si>
-    <t>H. DID URL Service Endpoint Transformation Use Cases (using "!" transformer (pipe) option and $serviceid transform option)</t>
-  </si>
-  <si>
     <t>Dereferencing a service-idto return the JSON description (fragment) of the service endpoint.</t>
   </si>
   <si>
@@ -213,12 +204,6 @@
     <t>4b2</t>
   </si>
   <si>
-    <t xml:space="preserve">
-did:xyz:1234!$serviceId="bops"
-did:xyz:1234!$serviceid="exam_svc"/foo/bar?a=1#flip
-</t>
-  </si>
-  <si>
     <t>did:xyz:1234!$contentId="hl:zQmWvQxTqbG2Z9HPJgG57jjwR154cKhbtJenbyYTWkjgF3e"</t>
   </si>
   <si>
@@ -232,16 +217,6 @@
   </si>
   <si>
     <t>http://uniresolver.io/did:xyz:1234did:xyz:1234!$exists="bops"</t>
-  </si>
-  <si>
-    <t>http://uniresolver.io/did:xyz:1234!$serviceid="bops"?
-http://uniresolver.io/did:xyz:1234!$serviceid="exam_svc"/foo/bar?a=1#flip</t>
-  </si>
-  <si>
-    <t>did:xyz:1234!$serviceid="bops"/foo/bar?a=1#flip</t>
-  </si>
-  <si>
-    <t>http://uniresolver.io/did:xyz:1234!serviceid="bops"/foo/bar?a=1#flip</t>
   </si>
   <si>
     <t>I. DID URL Service Endpoint Dereferencing Use Cases (using "$select" selectoroption)</t>
@@ -479,6 +454,31 @@
   </si>
   <si>
     <t>Not applicable</t>
+  </si>
+  <si>
+    <t>H. DID URL Service Endpoint Transformation Use Cases (using "!" transformer (pipe) option and $serviceId transform option)</t>
+  </si>
+  <si>
+    <t>http://uniresolver.io/did:xyz:1234!$serviceId="bops"?
+http://uniresolver.io/did:xyz:1234!$serviceId="exam_svc"/foo/bar?a=1#flip</t>
+  </si>
+  <si>
+    <t>Transform the DID URL using corresponding service endpoint using "!" pipe character and $serviceId transformation option (w/parameters)</t>
+  </si>
+  <si>
+    <t>did:xyz:1234!$serviceId="bops"/foo/bar?a=1#flip</t>
+  </si>
+  <si>
+    <t>http://uniresolver.io/did:xyz:1234!serviceId="bops"/foo/bar?a=1#flip</t>
+  </si>
+  <si>
+    <t>Transform the DID URL using corresponding service endpoint using "!" transformer (pipe) character and $serviceId transformation option (no parameters)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+did:xyz:1234!$serviceId="bops"
+did:xyz:1234!$serviceId="exam_svc"/foo/bar?a=1#flip
+</t>
   </si>
 </sst>
 </file>
@@ -611,11 +611,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -933,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA45131C-D45A-4CCB-AB34-792AD348A4B4}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,10 +996,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1010,10 +1010,10 @@
         <v>10</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1049,22 +1049,22 @@
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
@@ -1110,10 +1110,10 @@
         <v>28</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1132,10 +1132,10 @@
         <v>31</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1146,10 +1146,10 @@
         <v>32</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1160,10 +1160,10 @@
         <v>34</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1174,10 +1174,10 @@
         <v>35</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1188,10 +1188,10 @@
         <v>36</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1202,10 +1202,10 @@
         <v>37</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -1216,10 +1216,10 @@
         <v>38</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1238,10 +1238,10 @@
         <v>40</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1252,10 +1252,10 @@
         <v>41</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1263,21 +1263,21 @@
         <v>11</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
+      <c r="B31" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="13"/>
@@ -1300,10 +1300,10 @@
         <v>43</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1314,10 +1314,10 @@
         <v>45</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1328,10 +1328,10 @@
         <v>47</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1350,10 +1350,10 @@
         <v>50</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1364,43 +1364,43 @@
         <v>53</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -1411,32 +1411,32 @@
         <v>54</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>68</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>56</v>
+        <v>119</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>69</v>
+        <v>120</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>70</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
@@ -1444,35 +1444,35 @@
     </row>
     <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
@@ -1483,28 +1483,28 @@
         <v>18</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A27:D27"/>
     <mergeCell ref="A52:D52"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="A38:D38"/>
     <mergeCell ref="A44:D44"/>
     <mergeCell ref="A48:D48"/>
     <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A27:D27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>